<commit_message>
Reorganized test NMParserTest. Activated the main test
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\nmdataparser\enmexcelparser\src\test\resources\net\enanomapper\parser\testExcelParser\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2960" windowWidth="31860" windowHeight="15060"/>
+    <workbookView xWindow="2040" yWindow="2964" windowWidth="31860" windowHeight="15060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>NM</t>
   </si>
@@ -30,11 +35,17 @@
   <si>
     <t>NM-002</t>
   </si>
+  <si>
+    <t>NM-003</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,25 +410,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -432,12 +450,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Added test data in the excel file. Updated json config accordingly
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>NM</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>NM-001</t>
   </si>
@@ -40,13 +37,199 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>NM-Code</t>
+  </si>
+  <si>
+    <t>Conentration</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>owner-1</t>
+  </si>
+  <si>
+    <t>owner-2</t>
+  </si>
+  <si>
+    <t>owner-3</t>
+  </si>
+  <si>
+    <t>30 ppm</t>
+  </si>
+  <si>
+    <t>NM-Name</t>
+  </si>
+  <si>
+    <t>name-1</t>
+  </si>
+  <si>
+    <t>name-2</t>
+  </si>
+  <si>
+    <t>name-3</t>
+  </si>
+  <si>
+    <t>Public name</t>
+  </si>
+  <si>
+    <t>pname-1</t>
+  </si>
+  <si>
+    <t>pname-2</t>
+  </si>
+  <si>
+    <t>pname-3</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>var1-value</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>var2-001</t>
+  </si>
+  <si>
+    <t>var2-002</t>
+  </si>
+  <si>
+    <t>var2-003</t>
+  </si>
+  <si>
+    <t>Var3</t>
+  </si>
+  <si>
+    <t>var3-value</t>
+  </si>
+  <si>
+    <t>Citation title</t>
+  </si>
+  <si>
+    <t>title-1</t>
+  </si>
+  <si>
+    <t>title-2</t>
+  </si>
+  <si>
+    <t>title-3</t>
+  </si>
+  <si>
+    <t>Cit. year</t>
+  </si>
+  <si>
+    <t>Cit. owner</t>
+  </si>
+  <si>
+    <t>cit-own-1</t>
+  </si>
+  <si>
+    <t>cit-own-2</t>
+  </si>
+  <si>
+    <t>cit-own-3</t>
+  </si>
+  <si>
+    <t>Interpr-res</t>
+  </si>
+  <si>
+    <t>Interpret-crit</t>
+  </si>
+  <si>
+    <t>interp-res-1</t>
+  </si>
+  <si>
+    <t>interp-res-2</t>
+  </si>
+  <si>
+    <t>interp-res-3</t>
+  </si>
+  <si>
+    <t>interp-crit-1</t>
+  </si>
+  <si>
+    <t>interp-crit-2</t>
+  </si>
+  <si>
+    <t>interp-crit-3</t>
+  </si>
+  <si>
+    <t>Guide-1</t>
+  </si>
+  <si>
+    <t>guide1-01</t>
+  </si>
+  <si>
+    <t>guide1-02</t>
+  </si>
+  <si>
+    <t>guide1-03</t>
+  </si>
+  <si>
+    <t>Guide-2</t>
+  </si>
+  <si>
+    <t>guide2-01</t>
+  </si>
+  <si>
+    <t>guide2-02</t>
+  </si>
+  <si>
+    <t>guide2-03</t>
+  </si>
+  <si>
+    <t>Par1</t>
+  </si>
+  <si>
+    <t>Par2</t>
+  </si>
+  <si>
+    <t>1 K</t>
+  </si>
+  <si>
+    <t>2 K</t>
+  </si>
+  <si>
+    <t>3 K</t>
+  </si>
+  <si>
+    <t>par2-01</t>
+  </si>
+  <si>
+    <t>par2-02</t>
+  </si>
+  <si>
+    <t>par2-03</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>301 nm</t>
+  </si>
+  <si>
+    <t>302 nm</t>
+  </si>
+  <si>
+    <t>303 nm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +249,29 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,8 +301,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -166,7 +376,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,7 +411,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,36 +620,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2">
+        <v>2011</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3">
+        <v>2012</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4">
+        <v>2013</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -450,17 +857,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
+      <c r="A1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -476,6 +883,16 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added EXTERNAL_IDENTIFIERS in test resourses
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\nmdataparser\enmexcelparser\src\test\resources\net\enanomapper\parser\testExcelParser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\branches\nmdataparser\enmexcelparser\src\test\resources\net\enanomapper\parser\testExcelParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>NM-001</t>
   </si>
@@ -223,6 +223,30 @@
   </si>
   <si>
     <t>303 nm</t>
+  </si>
+  <si>
+    <t>ID1</t>
+  </si>
+  <si>
+    <t>id1-1</t>
+  </si>
+  <si>
+    <t>id1-2</t>
+  </si>
+  <si>
+    <t>id1-3</t>
+  </si>
+  <si>
+    <t>ID2</t>
+  </si>
+  <si>
+    <t>id2-1</t>
+  </si>
+  <si>
+    <t>id2-2</t>
+  </si>
+  <si>
+    <t>id2-3</t>
   </si>
 </sst>
 </file>
@@ -622,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,8 +672,12 @@
       <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
@@ -697,6 +725,12 @@
       <c r="E2" t="s">
         <v>18</v>
       </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
@@ -744,6 +778,12 @@
       <c r="E3" t="s">
         <v>19</v>
       </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
       <c r="I3" t="s">
         <v>31</v>
       </c>
@@ -790,6 +830,12 @@
       </c>
       <c r="E4" t="s">
         <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
       </c>
       <c r="I4" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Added testing for basic substance information
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>NM-001</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>id2-3</t>
+  </si>
+  <si>
+    <t>Reference subst</t>
+  </si>
+  <si>
+    <t>my-ref-subst</t>
   </si>
 </sst>
 </file>
@@ -647,7 +653,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,6 +884,9 @@
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -888,6 +897,9 @@
       </c>
       <c r="C10" t="s">
         <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for composition and properties
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>NM-001</t>
   </si>
@@ -253,6 +253,108 @@
   </si>
   <si>
     <t>my-ref-subst</t>
+  </si>
+  <si>
+    <t>StructureRelation</t>
+  </si>
+  <si>
+    <t>relation-1</t>
+  </si>
+  <si>
+    <t>relation-2</t>
+  </si>
+  <si>
+    <t>relation-3</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>content-1</t>
+  </si>
+  <si>
+    <t>content-2</t>
+  </si>
+  <si>
+    <t>content-3</t>
+  </si>
+  <si>
+    <t>format-1</t>
+  </si>
+  <si>
+    <t>format-2</t>
+  </si>
+  <si>
+    <t>format-3</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>formula-1</t>
+  </si>
+  <si>
+    <t>formula-2</t>
+  </si>
+  <si>
+    <t>formula-3</t>
+  </si>
+  <si>
+    <t>Smiles</t>
+  </si>
+  <si>
+    <t>CCC-1</t>
+  </si>
+  <si>
+    <t>CCC-2</t>
+  </si>
+  <si>
+    <t>CCC-3</t>
+  </si>
+  <si>
+    <t>InChI</t>
+  </si>
+  <si>
+    <t>inchi-1</t>
+  </si>
+  <si>
+    <t>inchi-2</t>
+  </si>
+  <si>
+    <t>inchi-3</t>
+  </si>
+  <si>
+    <t>InchiKey</t>
+  </si>
+  <si>
+    <t>inchi-key-1</t>
+  </si>
+  <si>
+    <t>inchi-key-2</t>
+  </si>
+  <si>
+    <t>inchi-key-3</t>
+  </si>
+  <si>
+    <t>property1</t>
+  </si>
+  <si>
+    <t>property2</t>
+  </si>
+  <si>
+    <t>prop1-1</t>
+  </si>
+  <si>
+    <t>prop1-2</t>
+  </si>
+  <si>
+    <t>prop1-3</t>
+  </si>
+  <si>
+    <t>property3</t>
   </si>
 </sst>
 </file>
@@ -650,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,7 +764,7 @@
     <col min="13" max="13" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -714,8 +816,38 @@
       <c r="R1" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -767,8 +899,38 @@
       <c r="R2" t="s">
         <v>63</v>
       </c>
+      <c r="S2" t="s">
+        <v>77</v>
+      </c>
+      <c r="T2" t="s">
+        <v>82</v>
+      </c>
+      <c r="U2" t="s">
+        <v>85</v>
+      </c>
+      <c r="V2" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" t="s">
+        <v>93</v>
+      </c>
+      <c r="X2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AB2">
+        <v>200.1</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -820,8 +982,38 @@
       <c r="R3" t="s">
         <v>64</v>
       </c>
+      <c r="S3" t="s">
+        <v>78</v>
+      </c>
+      <c r="T3" t="s">
+        <v>83</v>
+      </c>
+      <c r="U3" t="s">
+        <v>86</v>
+      </c>
+      <c r="V3" t="s">
+        <v>90</v>
+      </c>
+      <c r="W3" t="s">
+        <v>94</v>
+      </c>
+      <c r="X3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA3">
+        <v>5.2</v>
+      </c>
+      <c r="AB3">
+        <v>200.2</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -873,8 +1065,38 @@
       <c r="R4" t="s">
         <v>65</v>
       </c>
+      <c r="S4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T4" t="s">
+        <v>84</v>
+      </c>
+      <c r="U4" t="s">
+        <v>87</v>
+      </c>
+      <c r="V4" t="s">
+        <v>91</v>
+      </c>
+      <c r="W4" t="s">
+        <v>95</v>
+      </c>
+      <c r="X4" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA4">
+        <v>5.3</v>
+      </c>
+      <c r="AB4">
+        <v>200.3</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -888,7 +1110,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added effects info in test excel file
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="145">
   <si>
     <t>NM-001</t>
   </si>
@@ -355,6 +355,111 @@
   </si>
   <si>
     <t>property3</t>
+  </si>
+  <si>
+    <t>ProtocolEndpoint</t>
+  </si>
+  <si>
+    <t>pr-endpoint-1</t>
+  </si>
+  <si>
+    <t>pr-endpoint-2</t>
+  </si>
+  <si>
+    <t>pr-endpoint-3</t>
+  </si>
+  <si>
+    <t>Eff1</t>
+  </si>
+  <si>
+    <t>Cond11</t>
+  </si>
+  <si>
+    <t>Cond12</t>
+  </si>
+  <si>
+    <t>Eff2</t>
+  </si>
+  <si>
+    <t>Cond21</t>
+  </si>
+  <si>
+    <t>cond1-1</t>
+  </si>
+  <si>
+    <t>cond1-2</t>
+  </si>
+  <si>
+    <t>cond1-3</t>
+  </si>
+  <si>
+    <t>&lt;= 51 A</t>
+  </si>
+  <si>
+    <t>&lt;= 52 A</t>
+  </si>
+  <si>
+    <t>&lt;= 53 A</t>
+  </si>
+  <si>
+    <t>Eff3</t>
+  </si>
+  <si>
+    <t>1-56 Pa</t>
+  </si>
+  <si>
+    <t>2-56 Pa</t>
+  </si>
+  <si>
+    <t>3-56 Pa</t>
+  </si>
+  <si>
+    <t>~ 400 K</t>
+  </si>
+  <si>
+    <t>ca. 300 K</t>
+  </si>
+  <si>
+    <t>&gt; 200 K</t>
+  </si>
+  <si>
+    <t>Error1</t>
+  </si>
+  <si>
+    <t>101 m</t>
+  </si>
+  <si>
+    <t>102 m</t>
+  </si>
+  <si>
+    <t>103 m</t>
+  </si>
+  <si>
+    <t>&gt; 1</t>
+  </si>
+  <si>
+    <t>&gt; 2</t>
+  </si>
+  <si>
+    <t>&gt; 3</t>
+  </si>
+  <si>
+    <t>Eff4-Lo</t>
+  </si>
+  <si>
+    <t>Eff4-Unit</t>
+  </si>
+  <si>
+    <t>Eff4-Up</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>Eff4-Lo-Quil</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
   </si>
 </sst>
 </file>
@@ -433,12 +538,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -752,19 +860,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
     <col min="13" max="13" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -786,6 +895,9 @@
       <c r="G1" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
@@ -846,8 +958,41 @@
       <c r="AB1" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -869,6 +1014,9 @@
       <c r="G2" t="s">
         <v>71</v>
       </c>
+      <c r="H2" t="s">
+        <v>111</v>
+      </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
@@ -929,8 +1077,41 @@
       <c r="AB2">
         <v>200.1</v>
       </c>
+      <c r="AD2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>81</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK2">
+        <v>11</v>
+      </c>
+      <c r="AL2">
+        <v>21</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -952,6 +1133,9 @@
       <c r="G3" t="s">
         <v>72</v>
       </c>
+      <c r="H3" t="s">
+        <v>112</v>
+      </c>
       <c r="I3" t="s">
         <v>31</v>
       </c>
@@ -1012,8 +1196,41 @@
       <c r="AB3">
         <v>200.2</v>
       </c>
+      <c r="AD3" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>82</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK3">
+        <v>12</v>
+      </c>
+      <c r="AL3">
+        <v>22</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1035,6 +1252,9 @@
       <c r="G4" t="s">
         <v>73</v>
       </c>
+      <c r="H4" t="s">
+        <v>113</v>
+      </c>
       <c r="I4" t="s">
         <v>32</v>
       </c>
@@ -1095,8 +1315,41 @@
       <c r="AB4">
         <v>200.3</v>
       </c>
+      <c r="AD4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>83</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK4">
+        <v>13</v>
+      </c>
+      <c r="AL4">
+        <v>23</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1110,7 +1363,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added testing for protocol basic info
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="149">
   <si>
     <t>NM-001</t>
   </si>
@@ -460,6 +460,18 @@
   </si>
   <si>
     <t>&gt;=</t>
+  </si>
+  <si>
+    <t>Top category</t>
+  </si>
+  <si>
+    <t>Category code</t>
+  </si>
+  <si>
+    <t>my-category-code</t>
+  </si>
+  <si>
+    <t>test-top-cat</t>
   </si>
 </sst>
 </file>
@@ -862,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="AI4" sqref="AI4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1362,6 +1374,12 @@
       <c r="D9" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="E9" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1375,6 +1393,12 @@
       </c>
       <c r="D10" t="s">
         <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for citation and interpretation
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="152">
   <si>
     <t>NM-001</t>
   </si>
@@ -472,6 +472,15 @@
   </si>
   <si>
     <t>test-top-cat</t>
+  </si>
+  <si>
+    <t>year2011</t>
+  </si>
+  <si>
+    <t>year2012</t>
+  </si>
+  <si>
+    <t>year2013</t>
   </si>
 </sst>
 </file>
@@ -874,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,8 +1041,8 @@
       <c r="I2" t="s">
         <v>30</v>
       </c>
-      <c r="J2">
-        <v>2011</v>
+      <c r="J2" t="s">
+        <v>149</v>
       </c>
       <c r="K2" t="s">
         <v>35</v>
@@ -1151,8 +1160,8 @@
       <c r="I3" t="s">
         <v>31</v>
       </c>
-      <c r="J3">
-        <v>2012</v>
+      <c r="J3" t="s">
+        <v>150</v>
       </c>
       <c r="K3" t="s">
         <v>36</v>
@@ -1270,8 +1279,8 @@
       <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="J4">
-        <v>2013</v>
+      <c r="J4" t="s">
+        <v>151</v>
       </c>
       <c r="K4" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Added new testing function testEffectRecord()
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added test for effect eff1
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added test cases for eff2, eff3, eff4, eff5
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="161">
   <si>
     <t>NM-001</t>
   </si>
@@ -496,6 +496,18 @@
   </si>
   <si>
     <t>classification</t>
+  </si>
+  <si>
+    <t>Eff5</t>
+  </si>
+  <si>
+    <t>text-1</t>
+  </si>
+  <si>
+    <t>text-2</t>
+  </si>
+  <si>
+    <t>text-3</t>
   </si>
 </sst>
 </file>
@@ -913,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN10"/>
+  <dimension ref="A1:AO10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="AP4" sqref="AP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,7 +938,7 @@
     <col min="13" max="13" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1044,8 +1056,11 @@
       <c r="AN1" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AO1" s="1" t="s">
+        <v>157</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1163,8 +1178,11 @@
       <c r="AN2" t="s">
         <v>144</v>
       </c>
+      <c r="AO2" t="s">
+        <v>158</v>
+      </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1282,8 +1300,11 @@
       <c r="AN3" t="s">
         <v>144</v>
       </c>
+      <c r="AO3" t="s">
+        <v>159</v>
+      </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1401,13 +1422,16 @@
       <c r="AN4" t="s">
         <v>144</v>
       </c>
+      <c r="AO4" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="G8" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1433,7 +1457,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>